<commit_message>
Project StringExceptionBug is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/StringExceptionBug/StringExceptionBug.xlsx
+++ b/StringExceptionBug/StringExceptionBug.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Spreadsheet SpreadsheetResult mySpr1()</t>
   </si>
@@ -48,16 +48,26 @@
   </si>
   <si>
     <t>]</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult mySpr2()</t>
+  </si>
+  <si>
+    <t>]test</t>
+  </si>
+  <si>
+    <t>Stp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,7 +106,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -416,7 +426,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E88F1039-C3FE-6449-829C-E7A20C70B8B3}">
-  <dimension ref="C4:D6"/>
+  <dimension ref="B4:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:D6"/>
@@ -444,9 +454,30 @@
       </c>
       <c r="D6" s="2"/>
     </row>
+    <row r="8">
+      <c r="B8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>